<commit_message>
Update Les Proper Steam Engine Material List and Cost Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Les Proper Steam Engine/Parts List/Les Proper Steam Engine Material List and Cost Analysis.xlsx
+++ b/Les Proper Steam Engine/Parts List/Les Proper Steam Engine Material List and Cost Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tommy\Documents\Repositories\Steam-Engine\Les Proper Steam Engine\Parts List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CED10B-6BEE-48FE-A800-9C1F6ED5E107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1810D2B3-82F0-4EBC-97AA-41F3CD74FF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{3A7C17A1-F6D3-47ED-8154-3A4911587F59}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Parts List'!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -362,7 +363,7 @@
     <t>Brass Tubing, 3/16" OD, 0.032" Wall Thickness | McMaster-Carr</t>
   </si>
   <si>
-    <t>1/8" ID BRASS TUBE (3/32 OD)</t>
+    <t>1/8" ID BRASS TUBE</t>
   </si>
 </sst>
 </file>
@@ -424,12 +425,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -444,6 +439,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -467,20 +468,20 @@
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="12" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1096,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAE06AE-E5F1-46C1-A678-22AB2DDBD6F7}">
   <dimension ref="D1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1145,7 +1146,7 @@
       <c r="M3" t="s">
         <v>102</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="9">
         <f>SUM(M8:M36)</f>
         <v>136.63999999999999</v>
       </c>
@@ -1157,7 +1158,7 @@
       <c r="I4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <f>I4-1</f>
         <v>0.10000000000000009</v>
       </c>
@@ -1165,7 +1166,7 @@
       <c r="M4" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <f>N3/$I$2</f>
         <v>12.42181818181818</v>
       </c>
@@ -1225,7 +1226,7 @@
       <c r="D8" s="2">
         <v>1</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -1237,7 +1238,7 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <f>$I$4*H8*(G8+$I$3)</f>
         <v>0.74250000000000016</v>
       </c>
@@ -1247,7 +1248,7 @@
       <c r="K8" s="3">
         <v>2.76</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="11">
         <f>ROUNDUP(I8*$I$2/J8,0)</f>
         <v>1</v>
       </c>
@@ -1266,7 +1267,7 @@
       <c r="E9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="2">
@@ -1275,7 +1276,7 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <f t="shared" ref="I9:I16" si="0">$I$4*H9*(G9+$I$3)</f>
         <v>0.30250000000000005</v>
       </c>
@@ -1283,11 +1284,11 @@
         <v>1</v>
       </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="12">
+      <c r="L9" s="11">
         <f t="shared" ref="L9:L24" si="1">ROUNDUP(I9*$I$2/J9,0)</f>
         <v>4</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M9" s="15">
         <f t="shared" ref="M9:M24" si="2">K9*L9</f>
         <v>0</v>
       </c>
@@ -1309,7 +1310,7 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <f t="shared" si="0"/>
         <v>0.88550000000000018</v>
       </c>
@@ -1319,7 +1320,7 @@
       <c r="K10" s="3">
         <v>8.6999999999999993</v>
       </c>
-      <c r="L10" s="12">
+      <c r="L10" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1335,7 +1336,7 @@
       <c r="D11" s="2">
         <v>4</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="17" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -1347,7 +1348,7 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <f t="shared" si="0"/>
         <v>0.91849999999999998</v>
       </c>
@@ -1357,7 +1358,7 @@
       <c r="K11" s="3">
         <v>2.31</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1373,7 +1374,7 @@
       <c r="D12" s="2">
         <v>5</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="17" t="s">
         <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -1385,7 +1386,7 @@
       <c r="H12">
         <v>2</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <f t="shared" si="0"/>
         <v>1.837</v>
       </c>
@@ -1395,7 +1396,7 @@
       <c r="K12" s="3">
         <v>2.31</v>
       </c>
-      <c r="L12" s="12">
+      <c r="L12" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1411,7 +1412,7 @@
       <c r="D13" s="2">
         <v>6</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="17" t="s">
         <v>56</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -1423,7 +1424,7 @@
       <c r="H13">
         <v>4</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <f t="shared" si="0"/>
         <v>3.762</v>
       </c>
@@ -1433,7 +1434,7 @@
       <c r="K13" s="3">
         <v>1.42</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1461,7 +1462,7 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <f t="shared" si="0"/>
         <v>0.41250000000000003</v>
       </c>
@@ -1471,7 +1472,7 @@
       <c r="K14" s="3">
         <v>3.49</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1490,7 +1491,7 @@
       <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="2">
@@ -1499,7 +1500,7 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <f t="shared" si="0"/>
         <v>0.36849999999999999</v>
       </c>
@@ -1507,11 +1508,11 @@
         <v>1</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="12">
+      <c r="L15" s="11">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1533,7 +1534,7 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <f t="shared" si="0"/>
         <v>1.2375</v>
       </c>
@@ -1543,7 +1544,7 @@
       <c r="K16" s="3">
         <v>10.75</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="11">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1571,17 +1572,17 @@
       <c r="H17">
         <v>2</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <f t="shared" ref="I17:I25" si="3">$I$4*H17*(G17+$I$3)</f>
         <v>0.53900000000000003</v>
       </c>
       <c r="J17" s="2">
         <v>12</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="14">
         <v>6.25</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="D18" s="2">
         <v>10</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="17" t="s">
         <v>64</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -1606,17 +1607,17 @@
       <c r="H18">
         <v>8</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <f t="shared" si="3"/>
         <v>9.9</v>
       </c>
       <c r="J18" s="2">
         <v>100</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="10">
         <v>10.67</v>
       </c>
-      <c r="L18" s="12">
+      <c r="L18" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1635,7 +1636,7 @@
       <c r="E19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>66</v>
       </c>
       <c r="G19" s="2">
@@ -1644,7 +1645,7 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <f t="shared" si="3"/>
         <v>0.52249999999999996</v>
       </c>
@@ -1654,11 +1655,11 @@
       <c r="K19" s="2">
         <v>0</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="11">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1671,7 +1672,7 @@
       <c r="E20" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>66</v>
       </c>
       <c r="G20">
@@ -1680,7 +1681,7 @@
       <c r="H20">
         <v>1</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <f t="shared" si="3"/>
         <v>0.99550000000000016</v>
       </c>
@@ -1690,11 +1691,11 @@
       <c r="K20" s="2">
         <v>0</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="11">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1716,7 +1717,7 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <f t="shared" si="3"/>
         <v>1.0395000000000001</v>
       </c>
@@ -1726,7 +1727,7 @@
       <c r="K21" s="3">
         <v>1.32</v>
       </c>
-      <c r="L21" s="12">
+      <c r="L21" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1745,7 +1746,7 @@
       <c r="E22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>66</v>
       </c>
       <c r="G22" s="2">
@@ -1754,7 +1755,7 @@
       <c r="H22">
         <v>2</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <f t="shared" si="3"/>
         <v>0.27500000000000002</v>
       </c>
@@ -1764,11 +1765,11 @@
       <c r="K22" s="2">
         <v>0</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1790,7 +1791,7 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <f t="shared" si="3"/>
         <v>1.2375</v>
       </c>
@@ -1801,7 +1802,7 @@
       <c r="K23" s="3">
         <v>2.39</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="11">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1820,7 +1821,7 @@
       <c r="E24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G24" s="2">
@@ -1829,7 +1830,7 @@
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <f t="shared" si="3"/>
         <v>0.13750000000000001</v>
       </c>
@@ -1839,11 +1840,11 @@
       <c r="K24" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="12">
+      <c r="L24" s="11">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M24" s="16">
+      <c r="M24" s="15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1857,14 +1858,14 @@
       <c r="F25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="16">
         <f>I9+I15+I19+I20+I22+I24</f>
         <v>2.6015000000000001</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <f t="shared" si="3"/>
         <v>2.9991500000000002</v>
       </c>
@@ -1874,12 +1875,12 @@
       <c r="K25" s="3">
         <v>38.770000000000003</v>
       </c>
-      <c r="L25" s="12">
-        <f t="shared" ref="L25" si="4">ROUNDUP(I25*$I$2/J25,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M25" s="16">
-        <f t="shared" ref="M25" si="5">K25*L25</f>
+      <c r="L25" s="11">
+        <f>ROUNDUP(I25*$I$2/J25,0)</f>
+        <v>1</v>
+      </c>
+      <c r="M25" s="15">
+        <f>K25*L25</f>
         <v>38.770000000000003</v>
       </c>
       <c r="N25" s="1" t="s">
@@ -1891,21 +1892,21 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="12"/>
+      <c r="L26" s="11"/>
       <c r="M26" s="4"/>
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="4:14" x14ac:dyDescent="0.45">
       <c r="E27" s="2"/>
-      <c r="L27" s="12"/>
+      <c r="L27" s="11"/>
       <c r="M27" s="4"/>
     </row>
     <row r="28" spans="4:14" x14ac:dyDescent="0.45">
       <c r="E28" s="2"/>
-      <c r="L28" s="12"/>
+      <c r="L28" s="11"/>
       <c r="M28" s="4"/>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.45">
@@ -1915,20 +1916,20 @@
       <c r="G29" s="2"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
-      <c r="L29" s="12"/>
+      <c r="L29" s="11"/>
       <c r="M29" s="4"/>
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="L30" s="12"/>
+      <c r="L30" s="11"/>
       <c r="M30" s="4"/>
     </row>
     <row r="31" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="L31" s="12"/>
+      <c r="L31" s="11"/>
       <c r="M31" s="4"/>
     </row>
     <row r="32" spans="4:14" x14ac:dyDescent="0.45">
-      <c r="L32" s="12"/>
+      <c r="L32" s="11"/>
       <c r="M32" s="4"/>
     </row>
     <row r="35" spans="6:14" x14ac:dyDescent="0.45">
@@ -1940,14 +1941,14 @@
       <c r="F36" t="s">
         <v>92</v>
       </c>
-      <c r="K36" s="10">
+      <c r="K36" s="9">
         <v>6.76</v>
       </c>
       <c r="L36">
         <v>1</v>
       </c>
       <c r="M36" s="4">
-        <f t="shared" ref="M36" si="6">K36*L36</f>
+        <f>K36*L36</f>
         <v>6.76</v>
       </c>
       <c r="N36" s="1" t="s">

</xml_diff>